<commit_message>
Get Warranty info on computer
</commit_message>
<xml_diff>
--- a/asset_information/Hardware_assets.xlsx
+++ b/asset_information/Hardware_assets.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\psaini02\Desktop\Tufts Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\psaini02\Desktop\Tufts Testing\asset_information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB0750B-8347-4DF8-AE58-1CFB4EFA99E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{674CBC62-A49A-4C1C-86E8-FCC6056A1A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="37">
   <si>
     <t>Model ID</t>
   </si>
@@ -54,9 +54,6 @@
     <t>F4T8894</t>
   </si>
   <si>
-    <t>Dell Dell Pro Micro Plus QBM1251</t>
-  </si>
-  <si>
     <t>9YP8894</t>
   </si>
   <si>
@@ -72,19 +69,73 @@
     <t>98CGV94</t>
   </si>
   <si>
-    <t>Dell Dell Pro Micro Plus QBM1252</t>
-  </si>
-  <si>
-    <t>Dell Dell Pro Micro Plus QBM1253</t>
-  </si>
-  <si>
-    <t>Dell Dell Pro Micro Plus QBM1254</t>
-  </si>
-  <si>
-    <t>Dell Dell Pro Micro Plus QBM1255</t>
-  </si>
-  <si>
     <t>sschad01</t>
+  </si>
+  <si>
+    <t>8BCGV94</t>
+  </si>
+  <si>
+    <t>97CGV94</t>
+  </si>
+  <si>
+    <t>4GGGV94</t>
+  </si>
+  <si>
+    <t>C7D8894</t>
+  </si>
+  <si>
+    <t>D9CGV94</t>
+  </si>
+  <si>
+    <t>4BCGV94</t>
+  </si>
+  <si>
+    <t>4JGGV94</t>
+  </si>
+  <si>
+    <t>8FGGV94</t>
+  </si>
+  <si>
+    <t>4KGGV94</t>
+  </si>
+  <si>
+    <t>DBCGV94</t>
+  </si>
+  <si>
+    <t>CJGGV94</t>
+  </si>
+  <si>
+    <t>CDGGV94</t>
+  </si>
+  <si>
+    <t>5CCGV94</t>
+  </si>
+  <si>
+    <t>C8X8894</t>
+  </si>
+  <si>
+    <t>F3T8894</t>
+  </si>
+  <si>
+    <t>D9H8894</t>
+  </si>
+  <si>
+    <t>C9CGV94</t>
+  </si>
+  <si>
+    <t>9HGGV94</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Dell</t>
+  </si>
+  <si>
+    <t>QBM1250</t>
   </si>
 </sst>
 </file>
@@ -126,8 +177,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -146,9 +198,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CEC00EE3-0C93-4A40-BB87-A2C09AEFC2A8}" name="Table1" displayName="Table1" ref="A1:G7" totalsRowShown="0">
-  <autoFilter ref="A1:G7" xr:uid="{CEC00EE3-0C93-4A40-BB87-A2C09AEFC2A8}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CEC00EE3-0C93-4A40-BB87-A2C09AEFC2A8}" name="Table1" displayName="Table1" ref="A1:I25" totalsRowShown="0">
+  <autoFilter ref="A1:I25" xr:uid="{CEC00EE3-0C93-4A40-BB87-A2C09AEFC2A8}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{09810D7A-034A-43FE-BB39-8C08DEDF133A}" name="Model ID"/>
     <tableColumn id="2" xr3:uid="{DA95D237-714A-414C-9B7A-BF5565D72EBD}" name="Serial Number"/>
     <tableColumn id="3" xr3:uid="{07143435-DE00-4CA3-BC1A-550A1E01A38E}" name="Asset Tag"/>
@@ -156,6 +208,8 @@
     <tableColumn id="5" xr3:uid="{FFE427B1-9223-4761-A7C6-775136C606ED}" name="Assigned To"/>
     <tableColumn id="6" xr3:uid="{0F6AA0B7-059E-4AF1-8161-DE0D8DE7BCA5}" name="Warranty Start"/>
     <tableColumn id="7" xr3:uid="{CEF1677D-B89D-44B0-92CD-E7FB68BF4A70}" name="Warranty End"/>
+    <tableColumn id="8" xr3:uid="{87F252A6-C915-4437-A5B2-9FF2005B8234}" name="Manufacturer"/>
+    <tableColumn id="9" xr3:uid="{2B0B4D1F-A9E6-48D2-904F-5E75B58BE9FF}" name="Model"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -424,24 +478,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -463,8 +519,14 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -475,77 +537,521 @@
         <v>10367</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
       </c>
       <c r="C3">
         <v>10366</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>10368</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <v>10371</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6">
         <v>10369</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7">
         <v>10370</v>
       </c>
       <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>10372</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9">
+        <v>10374</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10">
+        <v>10373</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11">
+        <v>10365</v>
+      </c>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
         <v>19</v>
+      </c>
+      <c r="C12">
+        <v>10364</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>10363</v>
+      </c>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14">
+        <v>10385</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15">
+        <v>10383</v>
+      </c>
+      <c r="D15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16">
+        <v>10381</v>
+      </c>
+      <c r="D16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" t="s">
+        <v>35</v>
+      </c>
+      <c r="I16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17">
+        <v>10386</v>
+      </c>
+      <c r="D17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" t="s">
+        <v>35</v>
+      </c>
+      <c r="I17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18">
+        <v>10384</v>
+      </c>
+      <c r="D18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" t="s">
+        <v>35</v>
+      </c>
+      <c r="I18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19">
+        <v>10382</v>
+      </c>
+      <c r="D19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" t="s">
+        <v>35</v>
+      </c>
+      <c r="I19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20">
+        <v>10375</v>
+      </c>
+      <c r="D20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" t="s">
+        <v>35</v>
+      </c>
+      <c r="I20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21">
+        <v>10377</v>
+      </c>
+      <c r="D21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" t="s">
+        <v>35</v>
+      </c>
+      <c r="I21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22">
+        <v>10379</v>
+      </c>
+      <c r="D22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" t="s">
+        <v>35</v>
+      </c>
+      <c r="I22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23">
+        <v>10380</v>
+      </c>
+      <c r="D23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" t="s">
+        <v>35</v>
+      </c>
+      <c r="I23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24">
+        <v>10378</v>
+      </c>
+      <c r="D24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" t="s">
+        <v>35</v>
+      </c>
+      <c r="I24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25">
+        <v>10376</v>
+      </c>
+      <c r="D25" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" t="s">
+        <v>35</v>
+      </c>
+      <c r="I25" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create_record.py works with some test data
</commit_message>
<xml_diff>
--- a/asset_information/Hardware_assets.xlsx
+++ b/asset_information/Hardware_assets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4b6ffbbaaf6ffd3c/Desktop/Tufts/Tufts-Testing/asset_information/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\psaini02\Desktop\Tufts Testing\asset_information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_25D9ACA11012FD748F2513C8B030E1E95659B613" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D729D20-24D3-4AEE-BDBB-9E47B6D4F3C2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405E8461-89E6-4FEF-BDDE-826F7211C1A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5790" yWindow="4665" windowWidth="38700" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hardware Assets" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="35">
   <si>
     <t>Model ID</t>
   </si>
@@ -119,13 +119,19 @@
   </si>
   <si>
     <t>9HGGV94</t>
+  </si>
+  <si>
+    <t>06-09-2026</t>
+  </si>
+  <si>
+    <t>09-07-2029</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,6 +143,12 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -162,7 +174,9 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -181,50 +195,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -235,24 +206,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{03626EB9-9DC9-42B6-8FDC-C384CDD26F5C}" name="Table1" displayName="Table1" ref="A1:I19" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
-  <autoFilter ref="A1:I19" xr:uid="{03626EB9-9DC9-42B6-8FDC-C384CDD26F5C}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{0FD95E8B-4B25-47F5-B44F-BA26EF0B6BBD}" name="Model ID"/>
-    <tableColumn id="2" xr3:uid="{5C5A128B-63E0-4619-821B-AB6CC023E058}" name="Serial Number"/>
-    <tableColumn id="3" xr3:uid="{78578A0A-12C1-4D83-84EE-408664BAFC62}" name="Asset Tag"/>
-    <tableColumn id="4" xr3:uid="{163A03B6-C499-44C5-8674-FF013ACA18DB}" name="Managed By"/>
-    <tableColumn id="5" xr3:uid="{783F39E6-5E9F-4C92-AC5F-B22FC85E99F8}" name="Assigned To"/>
-    <tableColumn id="6" xr3:uid="{9BD15EB3-B907-4653-8724-05242FAC7FE1}" name="Warranty Start"/>
-    <tableColumn id="7" xr3:uid="{FBFA240B-0CEB-419E-A367-2FF3E345FC8B}" name="Warranty End"/>
-    <tableColumn id="8" xr3:uid="{1386E631-3F84-4347-B7AF-B9DF3CA44C85}" name="Manufacturer"/>
-    <tableColumn id="9" xr3:uid="{A8F67ADB-0A79-4096-B1C6-40BFA07A8F12}" name="Model"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -521,21 +474,10 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -632,10 +574,10 @@
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="G4" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="H4" t="s">
         <v>14</v>
@@ -1035,9 +977,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Created All Records (Except 3)
</commit_message>
<xml_diff>
--- a/asset_information/Hardware_assets.xlsx
+++ b/asset_information/Hardware_assets.xlsx
@@ -8,19 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\psaini02\Desktop\Tufts Testing\asset_information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405E8461-89E6-4FEF-BDDE-826F7211C1A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{637ED200-923A-47D2-986B-194A27310CAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30840" yWindow="795" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hardware Assets" sheetId="1" r:id="rId1"/>
+    <sheet name="Hardware Assets" sheetId="3" r:id="rId1"/>
+    <sheet name="Assets Done" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="39">
   <si>
     <t>Model ID</t>
   </si>
@@ -125,6 +139,18 @@
   </si>
   <si>
     <t>09-07-2029</t>
+  </si>
+  <si>
+    <t>Config Name</t>
+  </si>
+  <si>
+    <t>GVHOSL10379</t>
+  </si>
+  <si>
+    <t>GVHOSL10380</t>
+  </si>
+  <si>
+    <t>GVHOSL10376</t>
   </si>
 </sst>
 </file>
@@ -145,21 +171,33 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="8"/>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -174,28 +212,235 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="9">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -206,6 +451,46 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1B36D63C-3FF3-447B-B0F4-A384697494A1}" name="Table3" displayName="Table3" ref="A1:J4" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+  <autoFilter ref="A1:J4" xr:uid="{1B36D63C-3FF3-447B-B0F4-A384697494A1}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{F2E8C20A-290C-497E-BE65-E13E420E9D28}" name="Model ID"/>
+    <tableColumn id="2" xr3:uid="{BB3BCC26-A06D-400A-8FB3-82283EC175B5}" name="Serial Number"/>
+    <tableColumn id="3" xr3:uid="{E3D75037-6B3B-4E95-B047-AE9C7BE1BED9}" name="Asset Tag"/>
+    <tableColumn id="4" xr3:uid="{BC318388-B996-4688-98FC-F0FDF1F0D912}" name="Managed By"/>
+    <tableColumn id="5" xr3:uid="{2BC7096B-6082-463D-9D54-92E33EBA2B32}" name="Assigned To"/>
+    <tableColumn id="6" xr3:uid="{814B36B7-B3FB-4BA2-820A-40BDDBFFFB88}" name="Warranty Start"/>
+    <tableColumn id="7" xr3:uid="{F8EE0E09-B89E-4348-A5B5-09F2B150E6B1}" name="Warranty End"/>
+    <tableColumn id="8" xr3:uid="{24303657-12DE-433D-8CAD-717F6EB50E84}" name="Manufacturer"/>
+    <tableColumn id="9" xr3:uid="{8D376F36-6410-497F-95E9-923E33BC0142}" name="Model"/>
+    <tableColumn id="10" xr3:uid="{01C6D17A-E029-4CEA-9128-BAE6FF0FBC78}" name="Config Name"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7BD975FD-C624-4074-87DF-90E7C02C8D8E}" name="Table2" displayName="Table2" ref="A1:J16" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2" totalsRowBorderDxfId="1">
+  <autoFilter ref="A1:J16" xr:uid="{7BD975FD-C624-4074-87DF-90E7C02C8D8E}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{AC3E642F-F311-42B7-B13A-11C8D0645389}" name="Model ID"/>
+    <tableColumn id="2" xr3:uid="{2D7E4A37-B6C8-4212-9F4B-45C665378EE7}" name="Serial Number"/>
+    <tableColumn id="3" xr3:uid="{7198558D-6CE8-4739-ACE2-9440E594441D}" name="Asset Tag"/>
+    <tableColumn id="4" xr3:uid="{E1A65A72-8E36-4136-9678-CF37ED7352F0}" name="Managed By"/>
+    <tableColumn id="5" xr3:uid="{944E5903-E8F3-445D-8825-0D2F4C0BDB7F}" name="Assigned To"/>
+    <tableColumn id="6" xr3:uid="{7CB16162-1EA7-45FC-8EEB-FE4F130972C8}" name="Warranty Start"/>
+    <tableColumn id="7" xr3:uid="{4DD93245-D7A0-4E8F-9B4D-D10A96B74893}" name="Warranty End"/>
+    <tableColumn id="8" xr3:uid="{07A54C74-E405-4F92-B6F5-FFAE5736D899}" name="Manufacturer"/>
+    <tableColumn id="9" xr3:uid="{3D694C33-670C-4100-9236-08719A9D1AA9}" name="Model"/>
+    <tableColumn id="10" xr3:uid="{F89C2952-F885-485B-AAC7-E7218EB2C6C7}" name="Config Name" dataDxfId="0">
+      <calculatedColumnFormula>_xlfn.CONCAT("GVHOSL", Table2[[#This Row],[Asset Tag]])</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -470,16 +755,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E076CCF5-9420-4221-897B-329B257DF589}">
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -507,164 +804,349 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="J1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="5">
+        <v>10379</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="3">
+        <v>10380</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="9">
+        <v>10376</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66A3E4A3-454F-415B-BA68-685198425965}">
+  <dimension ref="A1:J16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="3">
         <v>10366</v>
       </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="6" t="str">
+        <f>_xlfn.CONCAT("GVHOSL", Table2[[#This Row],[Asset Tag]])</f>
+        <v>GVHOSL10366</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="5">
         <v>10371</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="D3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="6" t="str">
+        <f>_xlfn.CONCAT("GVHOSL", Table2[[#This Row],[Asset Tag]])</f>
+        <v>GVHOSL10371</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>10370</v>
       </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="H4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="6" t="str">
+        <f>_xlfn.CONCAT("GVHOSL", Table2[[#This Row],[Asset Tag]])</f>
+        <v>GVHOSL10370</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="5">
         <v>10372</v>
       </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="D5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="6" t="str">
+        <f>_xlfn.CONCAT("GVHOSL", Table2[[#This Row],[Asset Tag]])</f>
+        <v>GVHOSL10372</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <v>10374</v>
       </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="D6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="6" t="str">
+        <f>_xlfn.CONCAT("GVHOSL", Table2[[#This Row],[Asset Tag]])</f>
+        <v>GVHOSL10374</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="9">
         <v>10373</v>
       </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="6" t="str">
+        <f>_xlfn.CONCAT("GVHOSL", Table2[[#This Row],[Asset Tag]])</f>
+        <v>GVHOSL10373</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -689,8 +1171,12 @@
       <c r="I8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="6" t="str">
+        <f>_xlfn.CONCAT("GVHOSL", Table2[[#This Row],[Asset Tag]])</f>
+        <v>GVHOSL10365</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -715,8 +1201,12 @@
       <c r="I9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="6" t="str">
+        <f>_xlfn.CONCAT("GVHOSL", Table2[[#This Row],[Asset Tag]])</f>
+        <v>GVHOSL10364</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -741,8 +1231,12 @@
       <c r="I10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" s="6" t="str">
+        <f>_xlfn.CONCAT("GVHOSL", Table2[[#This Row],[Asset Tag]])</f>
+        <v>GVHOSL10363</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -767,8 +1261,12 @@
       <c r="I11" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" s="6" t="str">
+        <f>_xlfn.CONCAT("GVHOSL", Table2[[#This Row],[Asset Tag]])</f>
+        <v>GVHOSL10385</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -793,8 +1291,12 @@
       <c r="I12" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" s="6" t="str">
+        <f>_xlfn.CONCAT("GVHOSL", Table2[[#This Row],[Asset Tag]])</f>
+        <v>GVHOSL10383</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -819,8 +1321,12 @@
       <c r="I13" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" s="6" t="str">
+        <f>_xlfn.CONCAT("GVHOSL", Table2[[#This Row],[Asset Tag]])</f>
+        <v>GVHOSL10381</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -845,8 +1351,12 @@
       <c r="I14" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" s="6" t="str">
+        <f>_xlfn.CONCAT("GVHOSL", Table2[[#This Row],[Asset Tag]])</f>
+        <v>GVHOSL10384</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -871,113 +1381,46 @@
       <c r="I15" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="J15" s="6" t="str">
+        <f>_xlfn.CONCAT("GVHOSL", Table2[[#This Row],[Asset Tag]])</f>
+        <v>GVHOSL10382</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="10">
         <v>10377</v>
       </c>
-      <c r="D16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H16" t="s">
-        <v>14</v>
-      </c>
-      <c r="I16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17">
-        <v>10379</v>
-      </c>
-      <c r="D17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18">
-        <v>10380</v>
-      </c>
-      <c r="D18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" t="s">
-        <v>12</v>
-      </c>
-      <c r="G18" t="s">
-        <v>13</v>
-      </c>
-      <c r="H18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19">
-        <v>10376</v>
-      </c>
-      <c r="D19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" t="s">
-        <v>13</v>
-      </c>
-      <c r="H19" t="s">
-        <v>14</v>
-      </c>
-      <c r="I19" t="s">
-        <v>15</v>
+      <c r="D16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" s="6" t="str">
+        <f>_xlfn.CONCAT("GVHOSL", Table2[[#This Row],[Asset Tag]])</f>
+        <v>GVHOSL10377</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>